<commit_message>
feat: Add total price calculation and styling
</commit_message>
<xml_diff>
--- a/report_output.xlsx
+++ b/report_output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="My Report" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sales Report" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,13 +25,23 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004F81BD"/>
+        <bgColor rgb="004F81BD"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +56,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,28 +424,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>รายการสินค้า</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>ราคา (บาท)</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>จำนวน (ชิ้่น)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ราคารวม (บาท)</t>
         </is>
       </c>
     </row>
@@ -450,6 +470,9 @@
       <c r="C2" t="n">
         <v>2</v>
       </c>
+      <c r="D2" t="n">
+        <v>3000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -463,6 +486,9 @@
       <c r="C3" t="n">
         <v>5</v>
       </c>
+      <c r="D3" t="n">
+        <v>4750</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -475,6 +501,9 @@
       </c>
       <c r="C4" t="n">
         <v>10</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add Pandas pivot table script
</commit_message>
<xml_diff>
--- a/report_output.xlsx
+++ b/report_output.xlsx
@@ -9,7 +9,9 @@
   <sheets>
     <sheet name="Sales Report" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sales Report'!$A$1:$D$4</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -507,6 +509,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>